<commit_message>
Update Danh sách 63 tỉnh thành.xlsx
</commit_message>
<xml_diff>
--- a/Danh sách 63 tỉnh thành.xlsx
+++ b/Danh sách 63 tỉnh thành.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DS30_Hcmus\D.E\Nu_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F95BD5-650A-4C0E-ADE8-B59038C1DE61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4595CF9-A22B-4F1D-ACF3-A66899E51D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="82">
   <si>
     <t>Bắc bộ</t>
   </si>
@@ -280,9 +280,6 @@
   </si>
   <si>
     <t>id</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
 </sst>
 </file>
@@ -637,6 +634,16 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -657,16 +664,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -984,7 +981,7 @@
   <dimension ref="A1:V64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="C1" sqref="C1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="17.399999999999999" customHeight="1"/>
@@ -992,7 +989,7 @@
     <col min="1" max="1" width="18.44140625" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="38" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" style="28" customWidth="1"/>
     <col min="5" max="22" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1000,10 +997,10 @@
       <c r="A1" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="36"/>
+      <c r="D1" s="26"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1030,12 +1027,7 @@
       <c r="B2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C2">
-        <v>1585660</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>82</v>
-      </c>
+      <c r="D2" s="26"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -1062,12 +1054,7 @@
       <c r="B3" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C3">
-        <v>1584534</v>
-      </c>
-      <c r="D3" s="37" t="s">
-        <v>82</v>
-      </c>
+      <c r="D3" s="27"/>
     </row>
     <row r="4" spans="1:22" ht="17.399999999999999" customHeight="1">
       <c r="A4" s="15">
@@ -1076,9 +1063,7 @@
       <c r="B4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="37" t="s">
-        <v>82</v>
-      </c>
+      <c r="D4" s="27"/>
     </row>
     <row r="5" spans="1:22" ht="17.399999999999999" customHeight="1">
       <c r="A5" s="15">
@@ -1087,9 +1072,6 @@
       <c r="B5" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="38" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="6" spans="1:22" ht="17.399999999999999" customHeight="1">
       <c r="A6" s="15">
@@ -1098,9 +1080,7 @@
       <c r="B6" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="37" t="s">
-        <v>82</v>
-      </c>
+      <c r="D6" s="27"/>
     </row>
     <row r="7" spans="1:22" ht="17.399999999999999" customHeight="1">
       <c r="A7" s="15">
@@ -1109,9 +1089,6 @@
       <c r="B7" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="38" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="8" spans="1:22" ht="17.399999999999999" customHeight="1">
       <c r="A8" s="15">
@@ -1120,12 +1097,7 @@
       <c r="B8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C8">
-        <v>1587976</v>
-      </c>
-      <c r="D8" s="37" t="s">
-        <v>82</v>
-      </c>
+      <c r="D8" s="27"/>
     </row>
     <row r="9" spans="1:22" ht="17.399999999999999" customHeight="1">
       <c r="A9" s="15">
@@ -1134,12 +1106,6 @@
       <c r="B9" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C9">
-        <v>1568574</v>
-      </c>
-      <c r="D9" s="38" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="10" spans="1:22" ht="17.399999999999999" customHeight="1">
       <c r="A10">
@@ -1148,9 +1114,6 @@
       <c r="B10" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="38" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="11" spans="1:22" ht="17.399999999999999" customHeight="1">
       <c r="A11">
@@ -1159,9 +1122,7 @@
       <c r="B11" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="37" t="s">
-        <v>82</v>
-      </c>
+      <c r="D11" s="27"/>
     </row>
     <row r="12" spans="1:22" ht="17.399999999999999" customHeight="1">
       <c r="A12" s="15">
@@ -1170,12 +1131,7 @@
       <c r="B12" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C12">
-        <v>1577995</v>
-      </c>
-      <c r="D12" s="37" t="s">
-        <v>82</v>
-      </c>
+      <c r="D12" s="27"/>
     </row>
     <row r="13" spans="1:22" ht="17.399999999999999" customHeight="1">
       <c r="A13" s="15">
@@ -1184,9 +1140,7 @@
       <c r="B13" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="37" t="s">
-        <v>82</v>
-      </c>
+      <c r="D13" s="27"/>
     </row>
     <row r="14" spans="1:22" ht="17.399999999999999" customHeight="1">
       <c r="A14" s="15">
@@ -1195,12 +1149,7 @@
       <c r="B14" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="C14">
-        <v>1586203</v>
-      </c>
-      <c r="D14" s="37" t="s">
-        <v>82</v>
-      </c>
+      <c r="D14" s="27"/>
     </row>
     <row r="15" spans="1:22" ht="17.399999999999999" customHeight="1">
       <c r="A15" s="15">
@@ -1209,12 +1158,6 @@
       <c r="B15" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C15">
-        <v>1586185</v>
-      </c>
-      <c r="D15" s="38" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="16" spans="1:22" ht="17.399999999999999" customHeight="1">
       <c r="A16">
@@ -1223,32 +1166,24 @@
       <c r="B16" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="37" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="17.399999999999999" customHeight="1">
+      <c r="D16" s="27"/>
+    </row>
+    <row r="17" spans="1:3" ht="17.399999999999999" customHeight="1">
       <c r="A17" s="15">
         <v>1584169</v>
       </c>
       <c r="B17" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="C17">
-        <v>1586896</v>
-      </c>
-      <c r="D17" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="18" spans="1:3" ht="17.399999999999999" customHeight="1">
       <c r="A18" s="23"/>
       <c r="B18" s="24" t="s">
         <v>59</v>
       </c>
       <c r="C18" s="25"/>
     </row>
-    <row r="19" spans="1:4" ht="17.399999999999999" customHeight="1">
+    <row r="19" spans="1:3" ht="17.399999999999999" customHeight="1">
       <c r="A19" s="23">
         <v>1583477</v>
       </c>
@@ -1256,175 +1191,109 @@
         <v>62</v>
       </c>
       <c r="C19" s="25"/>
-      <c r="D19" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="20" spans="1:3" ht="17.399999999999999" customHeight="1">
       <c r="A20" s="15">
         <v>1582720</v>
       </c>
       <c r="B20" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="C20">
-        <v>1587923</v>
-      </c>
-      <c r="D20" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="21" spans="1:3" ht="17.399999999999999" customHeight="1">
       <c r="A21" s="15">
         <v>1582562</v>
       </c>
       <c r="B21" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="C21">
-        <v>1586151</v>
-      </c>
-      <c r="D21" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="22" spans="1:3" ht="17.399999999999999" customHeight="1">
       <c r="A22" s="15">
         <v>1581088</v>
       </c>
       <c r="B22" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="D22" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="23" spans="1:3" ht="17.399999999999999" customHeight="1">
       <c r="A23" s="15">
         <v>1581030</v>
       </c>
       <c r="B23" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C23">
-        <v>1581349</v>
-      </c>
-      <c r="D23" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="24" spans="1:3" ht="17.399999999999999" customHeight="1">
       <c r="A24" s="15">
         <v>1570449</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="25" spans="1:3" ht="17.399999999999999" customHeight="1">
       <c r="A25" s="15">
         <v>1581129</v>
       </c>
       <c r="B25" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C25">
-        <v>1581130</v>
-      </c>
-      <c r="D25" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="26" spans="1:3" ht="17.399999999999999" customHeight="1">
       <c r="A26" s="15">
         <v>1580700</v>
       </c>
       <c r="B26" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C26">
-        <v>1581047</v>
-      </c>
-      <c r="D26" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="27" spans="1:3" ht="17.399999999999999" customHeight="1">
       <c r="A27" s="15">
         <v>1581326</v>
       </c>
       <c r="B27" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="28" spans="1:3" ht="17.399999999999999" customHeight="1">
       <c r="A28" s="15">
         <v>1581297</v>
       </c>
       <c r="B28" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C28">
-        <v>1581298</v>
-      </c>
-      <c r="D28" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="29" spans="1:3" ht="17.399999999999999" customHeight="1">
       <c r="A29" s="15">
         <v>1570565</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="30" spans="1:3" ht="17.399999999999999" customHeight="1">
       <c r="A30" s="15">
         <v>1572594</v>
       </c>
       <c r="B30" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C30">
-        <v>1580830</v>
-      </c>
-      <c r="D30" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="31" spans="1:3" ht="17.399999999999999" customHeight="1">
       <c r="A31" s="15">
         <v>1580142</v>
       </c>
       <c r="B31" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="D31" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="32" spans="1:3" ht="17.399999999999999" customHeight="1">
       <c r="A32" s="15">
         <v>1579634</v>
       </c>
       <c r="B32" s="20" t="s">
         <v>39</v>
-      </c>
-      <c r="C32">
-        <v>1572151</v>
-      </c>
-      <c r="D32" s="38" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17.399999999999999" customHeight="1">
@@ -1434,9 +1303,6 @@
       <c r="B33" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="D33" s="38" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="34" spans="1:4" ht="17.399999999999999" customHeight="1">
       <c r="A34" s="15">
@@ -1445,12 +1311,6 @@
       <c r="B34" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="C34">
-        <v>1578500</v>
-      </c>
-      <c r="D34" s="38" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="35" spans="1:4" ht="17.399999999999999" customHeight="1">
       <c r="A35" s="15">
@@ -1459,9 +1319,6 @@
       <c r="B35" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="38" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="36" spans="1:4" ht="17.399999999999999" customHeight="1">
       <c r="A36" s="15">
@@ -1470,9 +1327,6 @@
       <c r="B36" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="D36" s="38" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="37" spans="1:4" ht="17.399999999999999" customHeight="1">
       <c r="A37" s="15">
@@ -1481,12 +1335,6 @@
       <c r="B37" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="C37">
-        <v>1576633</v>
-      </c>
-      <c r="D37" s="38" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="38" spans="1:4" ht="17.399999999999999" customHeight="1">
       <c r="A38" s="15">
@@ -1495,12 +1343,6 @@
       <c r="B38" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C38">
-        <v>1576303</v>
-      </c>
-      <c r="D38" s="38" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="39" spans="1:4" ht="17.399999999999999" customHeight="1">
       <c r="A39" s="15">
@@ -1509,9 +1351,7 @@
       <c r="B39" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="D39" s="37" t="s">
-        <v>82</v>
-      </c>
+      <c r="D39" s="27"/>
     </row>
     <row r="40" spans="1:4" ht="17.399999999999999" customHeight="1">
       <c r="A40" s="15">
@@ -1520,9 +1360,6 @@
       <c r="B40" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="D40" s="38" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="41" spans="1:4" ht="17.399999999999999" customHeight="1">
       <c r="A41" s="15">
@@ -1531,12 +1368,6 @@
       <c r="B41" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C41">
-        <v>1562798</v>
-      </c>
-      <c r="D41" s="38" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="42" spans="1:4" ht="17.399999999999999" customHeight="1">
       <c r="A42" s="15">
@@ -1545,12 +1376,6 @@
       <c r="B42" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="C42">
-        <v>1571968</v>
-      </c>
-      <c r="D42" s="38" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="43" spans="1:4" ht="17.399999999999999" customHeight="1">
       <c r="A43" s="15">
@@ -1559,9 +1384,6 @@
       <c r="B43" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="D43" s="38" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="44" spans="1:4" ht="17.399999999999999" customHeight="1">
       <c r="A44">
@@ -1570,9 +1392,7 @@
       <c r="B44" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D44" s="37" t="s">
-        <v>82</v>
-      </c>
+      <c r="D44" s="27"/>
     </row>
     <row r="45" spans="1:4" ht="17.399999999999999" customHeight="1">
       <c r="A45" s="15">
@@ -1581,12 +1401,6 @@
       <c r="B45" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C45">
-        <v>1569805</v>
-      </c>
-      <c r="D45" s="38" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="46" spans="1:4" ht="17.399999999999999" customHeight="1">
       <c r="A46" s="15">
@@ -1595,9 +1409,6 @@
       <c r="B46" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D46" s="38" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="47" spans="1:4" ht="17.399999999999999" customHeight="1">
       <c r="A47" s="15">
@@ -1606,9 +1417,6 @@
       <c r="B47" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D47" s="38" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="48" spans="1:4" ht="17.399999999999999" customHeight="1">
       <c r="A48" s="15">
@@ -1617,226 +1425,133 @@
       <c r="B48" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C48">
-        <v>1568770</v>
-      </c>
-      <c r="D48" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="49" spans="1:2" ht="17.399999999999999" customHeight="1">
       <c r="A49" s="15">
         <v>1568758</v>
       </c>
       <c r="B49" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C49">
-        <v>1580410</v>
-      </c>
-      <c r="D49" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="50" spans="1:2" ht="17.399999999999999" customHeight="1">
       <c r="A50" s="15">
         <v>1568733</v>
       </c>
       <c r="B50" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C50">
-        <v>1568738</v>
-      </c>
-      <c r="D50" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="51" spans="1:2" ht="17.399999999999999" customHeight="1">
       <c r="A51" s="15">
         <v>1559972</v>
       </c>
       <c r="B51" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C51">
-        <v>1567788</v>
-      </c>
-      <c r="D51" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="52" spans="1:2" ht="17.399999999999999" customHeight="1">
       <c r="A52" s="15">
         <v>1567643</v>
       </c>
       <c r="B52" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C52">
-        <v>1567681</v>
-      </c>
-      <c r="D52" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="53" spans="1:2" ht="17.399999999999999" customHeight="1">
       <c r="A53" s="15">
         <v>1566557</v>
       </c>
       <c r="B53" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="C53">
-        <v>1566559</v>
-      </c>
-      <c r="D53" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="54" spans="1:2" ht="17.399999999999999" customHeight="1">
       <c r="A54" s="15">
         <v>1566338</v>
       </c>
       <c r="B54" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C54">
-        <v>1566346</v>
-      </c>
-      <c r="D54" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="55" spans="1:2" ht="17.399999999999999" customHeight="1">
       <c r="A55" s="15">
         <v>1566319</v>
       </c>
       <c r="B55" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="D55" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="56" spans="1:2" ht="17.399999999999999" customHeight="1">
       <c r="A56" s="15">
         <v>1566165</v>
       </c>
       <c r="B56" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C56">
-        <v>1566166</v>
-      </c>
-      <c r="D56" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="57" spans="1:2" ht="17.399999999999999" customHeight="1">
       <c r="A57" s="15">
         <v>1580240</v>
       </c>
       <c r="B57" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C57">
-        <v>1565033</v>
-      </c>
-      <c r="D57" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="58" spans="1:2" ht="17.399999999999999" customHeight="1">
       <c r="A58">
         <v>1564676</v>
       </c>
       <c r="B58" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C58">
-        <v>1574023</v>
-      </c>
-      <c r="D58" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="59" spans="1:2" ht="17.399999999999999" customHeight="1">
       <c r="A59" s="15">
         <v>1566083</v>
       </c>
       <c r="B59" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C59">
-        <v>1580578</v>
-      </c>
-      <c r="D59" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="60" spans="1:2" ht="17.399999999999999" customHeight="1">
       <c r="A60" s="15">
         <v>1559975</v>
       </c>
       <c r="B60" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="C60">
-        <v>1563926</v>
-      </c>
-      <c r="D60" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="61" spans="1:2" ht="17.399999999999999" customHeight="1">
       <c r="A61" s="15">
         <v>1559976</v>
       </c>
       <c r="B61" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="C61">
-        <v>1563287</v>
-      </c>
-      <c r="D61" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="62" spans="1:2" ht="17.399999999999999" customHeight="1">
       <c r="A62" s="15">
         <v>1559977</v>
       </c>
       <c r="B62" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C62">
-        <v>1562693</v>
-      </c>
-      <c r="D62" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="63" spans="1:2" ht="17.399999999999999" customHeight="1">
       <c r="A63" s="22">
         <v>1562548</v>
       </c>
       <c r="B63" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="D63" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="64" spans="1:2" ht="17.399999999999999" customHeight="1">
       <c r="A64" s="15">
         <v>1559978</v>
       </c>
       <c r="B64" s="20" t="s">
         <v>73</v>
-      </c>
-      <c r="D64" s="38" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1868,36 +1583,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="34" t="s">
+      <c r="B1" s="39"/>
+      <c r="C1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="30" t="s">
+      <c r="D1" s="35"/>
+      <c r="E1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="H1" s="32" t="s">
+      <c r="F1" s="35"/>
+      <c r="H1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="33"/>
+      <c r="I1" s="37"/>
     </row>
     <row r="2" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="31"/>
+      <c r="C2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29" t="s">
+      <c r="D2" s="32"/>
+      <c r="E2" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="28"/>
+      <c r="F2" s="32"/>
       <c r="H2" s="19" t="s">
         <v>13</v>
       </c>
@@ -2054,10 +1769,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="27"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="16" t="s">
         <v>77</v>
       </c>
@@ -2244,10 +1959,10 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="27"/>
+      <c r="B19" s="31"/>
       <c r="C19" s="16" t="s">
         <v>80</v>
       </c>

</xml_diff>